<commit_message>
It was fixed parsers.
</commit_message>
<xml_diff>
--- a/src/main/resources/heroes.xlsx
+++ b/src/main/resources/heroes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>CREATURES</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t xml:space="preserve">5|(1&amp;2&amp;(3|(4&amp;(1^5|6&amp;47)|3)|(~89&amp;4|(42&amp;7)))|1) </t>
+  </si>
+  <si>
+    <t>SUPER HELL HOUND</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -458,45 +500,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -805,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,147 +839,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="25" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="30" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="17" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="18"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="26" t="s">
+      <c r="U2" s="31"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26" t="s">
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26" t="s">
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="26"/>
+      <c r="AB2" s="27"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="15" t="s">
+      <c r="I3" s="29"/>
+      <c r="J3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="13" t="s">
+      <c r="M3" s="23"/>
+      <c r="N3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="13" t="s">
+      <c r="O3" s="23"/>
+      <c r="P3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="15" t="s">
+      <c r="Q3" s="23"/>
+      <c r="R3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="16"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="23" t="s">
+      <c r="S3" s="29"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="X3" s="23" t="s">
+      <c r="X3" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="Y3" s="23" t="s">
+      <c r="Y3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="23" t="s">
+      <c r="Z3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AA3" s="23" t="s">
+      <c r="AA3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AB3" s="23" t="s">
+      <c r="AB3" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>18</v>
@@ -1040,12 +1043,12 @@
       <c r="V4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1259,12 +1262,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:V1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="AB3:AB4"/>
     <mergeCell ref="W1:AB1"/>
     <mergeCell ref="W2:X2"/>
@@ -1275,6 +1272,12 @@
     <mergeCell ref="Y3:Y4"/>
     <mergeCell ref="Z3:Z4"/>
     <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:V1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>

</xml_diff>

<commit_message>
I've added operation and begun work with writer.
</commit_message>
<xml_diff>
--- a/src/main/resources/heroes.xlsx
+++ b/src/main/resources/heroes.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
@@ -222,16 +220,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,119 +569,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="4" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="7"/>
+      <c r="S3" s="5"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
@@ -693,18 +691,18 @@
       <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
       <c r="R4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1335,10 +1333,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="K1:S1"/>
@@ -1355,34 +1349,12 @@
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
I've written some Test classes and fixed some problems with name and location.
</commit_message>
<xml_diff>
--- a/src/main/resources/heroes.xlsx
+++ b/src/main/resources/heroes.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
@@ -100,6 +100,9 @@
     <t>RED</t>
   </si>
   <si>
+    <t>SIMPLE SKELETON</t>
+  </si>
+  <si>
     <t>ORANGE</t>
   </si>
   <si>
@@ -125,9 +128,6 @@
   </si>
   <si>
     <t>GOLDEN</t>
-  </si>
-  <si>
-    <t>SIMPLE SKELETON</t>
   </si>
 </sst>
 </file>
@@ -217,9 +217,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -230,6 +227,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -539,149 +539,125 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" customWidth="1"/>
-    <col min="20" max="20" width="29.5703125" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" customWidth="1"/>
-    <col min="22" max="22" width="14" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="6" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="4"/>
+      <c r="M3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="5"/>
+      <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
@@ -691,18 +667,18 @@
       <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
       <c r="R4" s="1" t="s">
         <v>26</v>
       </c>
@@ -768,7 +744,7 @@
     </row>
     <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>95</v>
@@ -825,7 +801,7 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2">
         <v>60</v>
@@ -880,7 +856,7 @@
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -935,7 +911,7 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
@@ -990,7 +966,7 @@
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
@@ -1044,8 +1020,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>33</v>
+      <c r="A11" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="2">
         <f>2 * 3 * 4</f>
@@ -1162,7 +1138,7 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2">
         <v>155</v>
@@ -1217,7 +1193,7 @@
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2">
         <v>50</v>
@@ -1274,7 +1250,7 @@
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -1355,6 +1331,5 @@
     <mergeCell ref="N3:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>